<commit_message>
Updated guidance, fixed some references.
</commit_message>
<xml_diff>
--- a/output/nswhealthitocmedicationstatement.xlsx
+++ b/output/nswhealthitocmedicationstatement.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$70</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3019" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="348">
   <si>
     <t>Path</t>
   </si>
@@ -869,18 +869,6 @@
     <t>http://www.mims.com.au/codes</t>
   </si>
   <si>
-    <t>cerner</t>
-  </si>
-  <si>
-    <t>http://cerner.com/itoc/codes</t>
-  </si>
-  <si>
-    <t>imdsoft</t>
-  </si>
-  <si>
-    <t>http://www.imd-soft.com/itoc/codes</t>
-  </si>
-  <si>
     <t>MedicationStatement.medication[x].text</t>
   </si>
   <si>
@@ -908,7 +896,7 @@
     <t>medicationReference</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/StructureDefinition/au-medication)
+    <t xml:space="preserve">Reference(http://fhir.health.nsw.gov.au/fhir/ehealth/itoc/v1.0/StructureDefinition/nswhealthitocmedication)
 </t>
   </si>
   <si>
@@ -1271,7 +1259,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM86"/>
+  <dimension ref="A1:AM70"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -7775,11 +7763,9 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="B59" t="s" s="2">
         <v>270</v>
       </c>
+      <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
         <v>40</v>
       </c>
@@ -7800,19 +7786,19 @@
         <v>51</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>200</v>
+        <v>271</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>201</v>
+        <v>272</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>203</v>
+        <v>274</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>40</v>
@@ -7861,13 +7847,13 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>205</v>
+        <v>275</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>40</v>
@@ -7879,20 +7865,22 @@
         <v>40</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>206</v>
+        <v>276</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>207</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="B60" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>278</v>
+      </c>
       <c r="C60" t="s" s="2">
         <v>40</v>
       </c>
@@ -7910,18 +7898,20 @@
         <v>40</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>52</v>
+        <v>279</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>189</v>
+        <v>280</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M60" s="2"/>
+        <v>177</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>178</v>
+      </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>40</v>
@@ -7970,10 +7960,10 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>50</v>
@@ -7982,16 +7972,16 @@
         <v>40</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>40</v>
+        <v>183</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>40</v>
@@ -7999,18 +7989,18 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>213</v>
+        <v>281</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>40</v>
@@ -8019,20 +8009,18 @@
         <v>40</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>95</v>
+        <v>282</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>194</v>
+        <v>283</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>122</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>40</v>
@@ -8069,48 +8057,48 @@
         <v>40</v>
       </c>
       <c r="AA61" t="s" s="2">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="AB61" t="s" s="2">
-        <v>196</v>
+        <v>40</v>
       </c>
       <c r="AC61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD61" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>197</v>
+        <v>281</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>40</v>
+        <v>285</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>192</v>
+        <v>286</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>40</v>
+        <v>287</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>40</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>214</v>
+        <v>289</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8118,7 +8106,7 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F62" t="s" s="2">
         <v>50</v>
@@ -8133,26 +8121,22 @@
         <v>51</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>64</v>
+        <v>290</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>215</v>
+        <v>291</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>218</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" t="s" s="2">
-        <v>271</v>
+        <v>40</v>
       </c>
       <c r="R62" t="s" s="2">
         <v>40</v>
@@ -8194,7 +8178,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>220</v>
+        <v>289</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8209,21 +8193,21 @@
         <v>62</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>40</v>
+        <v>293</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>222</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>223</v>
+        <v>295</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8246,16 +8230,16 @@
         <v>51</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>52</v>
+        <v>296</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>224</v>
+        <v>297</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>226</v>
+        <v>299</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8305,7 +8289,7 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
@@ -8320,21 +8304,21 @@
         <v>62</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>40</v>
+        <v>300</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>228</v>
+        <v>301</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>40</v>
+        <v>302</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>229</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8357,18 +8341,16 @@
         <v>51</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>70</v>
+        <v>304</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>231</v>
+        <v>305</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="M64" s="2"/>
-      <c r="N64" t="s" s="2">
-        <v>233</v>
-      </c>
+      <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>40</v>
       </c>
@@ -8416,7 +8398,7 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>234</v>
+        <v>303</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8434,18 +8416,18 @@
         <v>40</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>235</v>
+        <v>307</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>40</v>
+        <v>308</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>236</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>237</v>
+        <v>309</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8465,21 +8447,19 @@
         <v>40</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>52</v>
+        <v>310</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>238</v>
+        <v>311</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>239</v>
+        <v>312</v>
       </c>
       <c r="M65" s="2"/>
-      <c r="N65" t="s" s="2">
-        <v>240</v>
-      </c>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8527,7 +8507,7 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>241</v>
+        <v>309</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8545,18 +8525,18 @@
         <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>242</v>
+        <v>313</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>40</v>
+        <v>314</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>243</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>244</v>
+        <v>315</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8567,7 +8547,7 @@
         <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>40</v>
@@ -8576,23 +8556,21 @@
         <v>40</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>245</v>
+        <v>316</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>246</v>
+        <v>317</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>247</v>
+        <v>318</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>249</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>40</v>
       </c>
@@ -8640,13 +8618,13 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>250</v>
+        <v>315</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>40</v>
@@ -8658,22 +8636,20 @@
         <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>251</v>
+        <v>320</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>252</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="B67" t="s" s="2">
-        <v>272</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
         <v>40</v>
       </c>
@@ -8682,7 +8658,7 @@
         <v>41</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>40</v>
@@ -8691,23 +8667,21 @@
         <v>40</v>
       </c>
       <c r="I67" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>200</v>
+        <v>322</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>201</v>
+        <v>323</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>40</v>
       </c>
@@ -8731,13 +8705,11 @@
         <v>40</v>
       </c>
       <c r="W67" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X67" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="X67" s="2"/>
       <c r="Y67" t="s" s="2">
-        <v>40</v>
+        <v>325</v>
       </c>
       <c r="Z67" t="s" s="2">
         <v>40</v>
@@ -8755,7 +8727,7 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>205</v>
+        <v>321</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -8770,21 +8742,21 @@
         <v>62</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>40</v>
+        <v>326</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>206</v>
+        <v>327</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>40</v>
+        <v>328</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>207</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>212</v>
+        <v>329</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8795,7 +8767,7 @@
         <v>41</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>40</v>
@@ -8807,15 +8779,17 @@
         <v>40</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>52</v>
+        <v>330</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>189</v>
+        <v>331</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M68" s="2"/>
+        <v>332</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
         <v>40</v>
@@ -8864,28 +8838,28 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>191</v>
+        <v>329</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>40</v>
+        <v>334</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>192</v>
+        <v>335</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>40</v>
+        <v>328</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>40</v>
@@ -8893,11 +8867,11 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>213</v>
+        <v>336</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
@@ -8916,17 +8890,15 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>95</v>
+        <v>337</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>194</v>
+        <v>338</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>122</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="M69" s="2"/>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>40</v>
@@ -8963,19 +8935,19 @@
         <v>40</v>
       </c>
       <c r="AA69" t="s" s="2">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="AB69" t="s" s="2">
-        <v>196</v>
+        <v>40</v>
       </c>
       <c r="AC69" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD69" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>197</v>
+        <v>336</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -8987,13 +8959,13 @@
         <v>40</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>192</v>
+        <v>341</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>40</v>
@@ -9004,7 +8976,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>214</v>
+        <v>342</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9012,10 +8984,10 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>40</v>
@@ -9024,29 +8996,27 @@
         <v>40</v>
       </c>
       <c r="I70" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>64</v>
+        <v>343</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>216</v>
+        <v>345</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>218</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" t="s" s="2">
-        <v>273</v>
+        <v>40</v>
       </c>
       <c r="R70" t="s" s="2">
         <v>40</v>
@@ -9088,13 +9058,13 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>220</v>
+        <v>342</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>40</v>
@@ -9106,1787 +9076,17 @@
         <v>40</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>221</v>
+        <v>347</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="71" hidden="true">
-      <c r="A71" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F71" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J71" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="K71" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="N71" s="2"/>
-      <c r="O71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P71" s="2"/>
-      <c r="Q71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AF71" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG71" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI71" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM71" t="s" s="2">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="72" hidden="true">
-      <c r="A72" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F72" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="M72" s="2"/>
-      <c r="N72" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="O72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P72" s="2"/>
-      <c r="Q72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="AL72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM72" t="s" s="2">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="73" hidden="true">
-      <c r="A73" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F73" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I73" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J73" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="K73" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="M73" s="2"/>
-      <c r="N73" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="O73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P73" s="2"/>
-      <c r="Q73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="74" hidden="true">
-      <c r="A74" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F74" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P74" s="2"/>
-      <c r="Q74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="75" hidden="true">
-      <c r="A75" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F75" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P75" s="2"/>
-      <c r="Q75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="76" hidden="true">
-      <c r="A76" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="B76" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="C76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F76" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J76" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="K76" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="N76" s="2"/>
-      <c r="O76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P76" s="2"/>
-      <c r="Q76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" hidden="true">
-      <c r="A77" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="F77" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J77" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="K77" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P77" s="2"/>
-      <c r="Q77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="78" hidden="true">
-      <c r="A78" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D78" s="2"/>
-      <c r="E78" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F78" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J78" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="K78" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P78" s="2"/>
-      <c r="Q78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE78" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="AF78" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG78" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI78" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ78" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="79" hidden="true">
-      <c r="A79" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="B79" s="2"/>
-      <c r="C79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F79" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I79" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J79" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="K79" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="N79" s="2"/>
-      <c r="O79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P79" s="2"/>
-      <c r="Q79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE79" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="AF79" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG79" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI79" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ79" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="AM79" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" hidden="true">
-      <c r="A80" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F80" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I80" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="J80" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="K80" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P80" s="2"/>
-      <c r="Q80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE80" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="AF80" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG80" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI80" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK80" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="AL80" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="AM80" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="81" hidden="true">
-      <c r="A81" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="B81" s="2"/>
-      <c r="C81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F81" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J81" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="K81" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="L81" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="M81" s="2"/>
-      <c r="N81" s="2"/>
-      <c r="O81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P81" s="2"/>
-      <c r="Q81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE81" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="AF81" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI81" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK81" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AL81" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="AM81" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" hidden="true">
-      <c r="A82" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="B82" s="2"/>
-      <c r="C82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D82" s="2"/>
-      <c r="E82" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F82" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J82" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="K82" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="L82" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="N82" s="2"/>
-      <c r="O82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P82" s="2"/>
-      <c r="Q82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE82" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="AF82" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG82" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI82" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK82" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="AL82" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM82" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" hidden="true">
-      <c r="A83" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D83" s="2"/>
-      <c r="E83" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F83" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J83" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="K83" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="N83" s="2"/>
-      <c r="O83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P83" s="2"/>
-      <c r="Q83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W83" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X83" s="2"/>
-      <c r="Y83" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="Z83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE83" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="AF83" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG83" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI83" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ83" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="AK83" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="AL83" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="AM83" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="84" hidden="true">
-      <c r="A84" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="B84" s="2"/>
-      <c r="C84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="E84" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F84" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J84" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="K84" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="L84" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N84" s="2"/>
-      <c r="O84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P84" s="2"/>
-      <c r="Q84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE84" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="AF84" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG84" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH84" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI84" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ84" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="AK84" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="AL84" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="AM84" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="85" hidden="true">
-      <c r="A85" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="B85" s="2"/>
-      <c r="C85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D85" s="2"/>
-      <c r="E85" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F85" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J85" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="K85" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="L85" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P85" s="2"/>
-      <c r="Q85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE85" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="AF85" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG85" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI85" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ85" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="AK85" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="AL85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM85" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="86" hidden="true">
-      <c r="A86" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="B86" s="2"/>
-      <c r="C86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D86" s="2"/>
-      <c r="E86" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F86" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="J86" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="K86" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="L86" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="M86" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="N86" s="2"/>
-      <c r="O86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P86" s="2"/>
-      <c r="Q86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE86" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="AF86" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG86" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI86" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="AJ86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK86" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="AL86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM86" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM86">
+  <autoFilter ref="A1:AM70">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10896,7 +9096,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI85">
+  <conditionalFormatting sqref="A2:AI69">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>